<commit_message>
More progress on incommute work
</commit_message>
<xml_diff>
--- a/applications/travel_model_lu_inputs/2015/Employment/2012-2016 CTPP Places to Superdistrict Equivalency.xlsx
+++ b/applications/travel_model_lu_inputs/2015/Employment/2012-2016 CTPP Places to Superdistrict Equivalency.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Read Me" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="468">
   <si>
     <t>0600135</t>
   </si>
@@ -1426,6 +1426,9 @@
   </si>
   <si>
     <t xml:space="preserve">The Comp_SD Incommute Equivalence tab represents the respective shares of the total incommuters by composite superdistrict grouping. For example, the group of TAZs within the composite superdistrict group 8_9_10_11_12_13 account for 32.5 percent of all incommuters. </t>
+  </si>
+  <si>
+    <t>Share_Incommute</t>
   </si>
 </sst>
 </file>
@@ -1782,7 +1785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -7348,8 +7351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7363,7 +7366,7 @@
         <v>225</v>
       </c>
       <c r="B1" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>